<commit_message>
added spanish meeting and link made study schedule 3 fixed the mp3 play thing on the pomodoro
</commit_message>
<xml_diff>
--- a/StudySchedule3.xlsx
+++ b/StudySchedule3.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\small-python-projects\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4812F5-AE9B-43F2-9FC3-687142049389}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
   <si>
     <t>('Chemistry', 'Math')</t>
   </si>
@@ -98,13 +104,34 @@
   </si>
   <si>
     <t>('Lit', 'Add Math')</t>
+  </si>
+  <si>
+    <t>mon</t>
+  </si>
+  <si>
+    <t>tue</t>
+  </si>
+  <si>
+    <t>wed</t>
+  </si>
+  <si>
+    <t>thu</t>
+  </si>
+  <si>
+    <t>fri</t>
+  </si>
+  <si>
+    <t>sat</t>
+  </si>
+  <si>
+    <t>sun</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,13 +139,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -133,14 +172,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -187,7 +235,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -219,9 +267,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -253,6 +319,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -428,238 +512,337 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="D18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="D22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>25</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="D25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>26</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>27</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>28</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
+      <c r="D28" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>